<commit_message>
Creating notebook for ff and OEW offset
</commit_message>
<xml_diff>
--- a/Data/A320_inputs.xlsx
+++ b/Data/A320_inputs.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parolin\Aeco\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giparoli\Documents\Projetos\AEco\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1C78AD-2613-4166-B176-6B676BBC398F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC492D32-BC10-4566-A32A-7B49CD6DFC0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A320" sheetId="2" r:id="rId1"/>
     <sheet name="A320_old" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,155 +47,74 @@
   <commentList>
     <comment ref="C17" authorId="0" shapeId="0" xr:uid="{396ABCAF-54DB-4DB7-9877-C4D9CB0C752F}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     107087 kWh/month @ G1170. Considering 500 workers in the building, the average per worker is 214.17.</t>
-        </r>
       </text>
     </comment>
     <comment ref="C18" authorId="1" shapeId="0" xr:uid="{DB4559B8-B4D5-46B7-9443-71ECDC1325D0}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     190 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 0.38</t>
-        </r>
       </text>
     </comment>
     <comment ref="C19" authorId="2" shapeId="0" xr:uid="{7E0439F0-61E6-4462-942E-D17301560662}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     750 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 1.5</t>
-        </r>
       </text>
     </comment>
     <comment ref="C42" authorId="3" shapeId="0" xr:uid="{0DC24375-CA62-42B7-82D8-58C5246FFD6F}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     80000 kWh/month @ G1360. Considering 18000 m², the average per m² is 4.44</t>
-        </r>
       </text>
     </comment>
     <comment ref="C43" authorId="4" shapeId="0" xr:uid="{72D2B639-7D47-4D26-A14C-D414C3B25E87}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     80 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00444</t>
-        </r>
       </text>
     </comment>
     <comment ref="C44" authorId="5" shapeId="0" xr:uid="{B1C3D0ED-7599-4C92-8848-AD9F3F4ACEF7}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     64 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00356</t>
-        </r>
       </text>
     </comment>
     <comment ref="C45" authorId="6" shapeId="0" xr:uid="{B5C3BFB3-019D-426D-A008-79A436013E7A}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     0.27 m³/month @ G1360. Considering 18000 m², the average per m² is 0.000015</t>
-        </r>
       </text>
     </comment>
     <comment ref="C52" authorId="7" shapeId="0" xr:uid="{56892021-C2EB-47AE-B836-157999D31257}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     rome fiumicino</t>
-        </r>
       </text>
     </comment>
     <comment ref="C53" authorId="8" shapeId="0" xr:uid="{8A1481D7-3873-420A-9E14-35507B0A9525}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     rome fiumicino</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -205,168 +124,87 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={396ABCAF-54DB-4DB7-9877-C4D9CB0C752F}</author>
-    <author>tc={DB4559B8-B4D5-46B7-9443-71ECDC1325D0}</author>
-    <author>tc={7E0439F0-61E6-4462-942E-D17301560662}</author>
-    <author>tc={0DC24375-CA62-42B7-82D8-58C5246FFD6F}</author>
-    <author>tc={72D2B639-7D47-4D26-A14C-D414C3B25E87}</author>
-    <author>tc={B1C3D0ED-7599-4C92-8848-AD9F3F4ACEF7}</author>
-    <author>tc={B5C3BFB3-019D-426D-A008-79A436013E7A}</author>
-    <author>tc={56892021-C2EB-47AE-B836-157999D31257}</author>
-    <author>tc={8A1481D7-3873-420A-9E14-35507B0A9525}</author>
+    <author>tc={396ABCAF-54DB-4DB8-9877-C4D9CB0C752F}</author>
+    <author>tc={DB4559B8-B4D5-46B8-9443-71ECDC1325D0}</author>
+    <author>tc={7E0439F0-61E6-4463-942E-D17301560662}</author>
+    <author>tc={0DC24375-CA62-42B8-82D8-58C5246FFD6F}</author>
+    <author>tc={72D2B639-7D47-4D27-A14C-D414C3B25E87}</author>
+    <author>tc={B1C3D0ED-7599-4C93-8848-AD9F3F4ACEF7}</author>
+    <author>tc={B5C3BFB3-019D-426E-A008-79A436013E7A}</author>
+    <author>tc={56892021-C2EB-47AF-B836-157999D31257}</author>
+    <author>tc={8A1481D7-3873-420B-9E14-35507B0A9525}</author>
   </authors>
   <commentList>
     <comment ref="C18" authorId="0" shapeId="0" xr:uid="{9DCAD449-515F-4C52-A81B-9DD0645F96A0}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     107087 kWh/month @ G1170. Considering 500 workers in the building, the average per worker is 214.17.</t>
-        </r>
       </text>
     </comment>
     <comment ref="C19" authorId="1" shapeId="0" xr:uid="{A8376446-BA5A-474E-B1DE-A62EAF0D480B}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     190 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 0.38</t>
-        </r>
       </text>
     </comment>
     <comment ref="C20" authorId="2" shapeId="0" xr:uid="{B6B9048D-2491-4A87-AB9B-F417765EA6EB}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     750 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 1.5</t>
-        </r>
       </text>
     </comment>
     <comment ref="C44" authorId="3" shapeId="0" xr:uid="{282687E6-1418-4591-8238-428E5128F81E}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     80000 kWh/month @ G1360. Considering 18000 m², the average per m² is 4.44</t>
-        </r>
       </text>
     </comment>
     <comment ref="C45" authorId="4" shapeId="0" xr:uid="{EA130BB8-A62F-4FF1-ABC4-D638911F80ED}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     80 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00444</t>
-        </r>
       </text>
     </comment>
     <comment ref="C46" authorId="5" shapeId="0" xr:uid="{3516DB52-47B4-409B-BE71-020DB43D759E}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     64 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00356</t>
-        </r>
       </text>
     </comment>
     <comment ref="C47" authorId="6" shapeId="0" xr:uid="{F05268AD-D18B-4870-B6EF-1CD8A55B47F0}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     0.27 m³/month @ G1360. Considering 18000 m², the average per m² is 0.000015</t>
-        </r>
       </text>
     </comment>
     <comment ref="C54" authorId="7" shapeId="0" xr:uid="{BE43428D-298F-4012-A900-46220528227B}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     rome fiumicino</t>
-        </r>
       </text>
     </comment>
     <comment ref="C55" authorId="8" shapeId="0" xr:uid="{D1A7C9D6-2DA9-4369-8642-1EB919E028E2}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     rome fiumicino</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -1703,31 +1541,63 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C18" dT="2019-12-31T13:50:55.89" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{396ABCAF-54DB-4DB7-9877-C4D9CB0C752F}">
+  <threadedComment ref="C17" dT="2019-12-31T13:50:55.89" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{396ABCAF-54DB-4DB7-9877-C4D9CB0C752F}">
     <text>107087 kWh/month @ G1170. Considering 500 workers in the building, the average per worker is 214.17.</text>
   </threadedComment>
-  <threadedComment ref="C19" dT="2019-12-31T14:01:21.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{DB4559B8-B4D5-46B7-9443-71ECDC1325D0}">
+  <threadedComment ref="C18" dT="2019-12-31T14:01:21.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{DB4559B8-B4D5-46B7-9443-71ECDC1325D0}">
     <text>190 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 0.38</text>
   </threadedComment>
-  <threadedComment ref="C20" dT="2019-12-31T14:02:51.19" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{7E0439F0-61E6-4462-942E-D17301560662}">
+  <threadedComment ref="C19" dT="2019-12-31T14:02:51.19" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{7E0439F0-61E6-4462-942E-D17301560662}">
     <text>750 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 1.5</text>
   </threadedComment>
-  <threadedComment ref="C44" dT="2019-12-31T14:53:25.54" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{0DC24375-CA62-42B7-82D8-58C5246FFD6F}">
+  <threadedComment ref="C42" dT="2019-12-31T14:53:25.54" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{0DC24375-CA62-42B7-82D8-58C5246FFD6F}">
     <text>80000 kWh/month @ G1360. Considering 18000 m², the average per m² is 4.44</text>
   </threadedComment>
-  <threadedComment ref="C45" dT="2019-12-31T14:55:29.34" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{72D2B639-7D47-4D26-A14C-D414C3B25E87}">
+  <threadedComment ref="C43" dT="2019-12-31T14:55:29.34" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{72D2B639-7D47-4D26-A14C-D414C3B25E87}">
     <text>80 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00444</text>
   </threadedComment>
-  <threadedComment ref="C46" dT="2019-12-31T16:34:31.50" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{B1C3D0ED-7599-4C92-8848-AD9F3F4ACEF7}">
+  <threadedComment ref="C44" dT="2019-12-31T16:34:31.50" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{B1C3D0ED-7599-4C92-8848-AD9F3F4ACEF7}">
     <text>64 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00356</text>
   </threadedComment>
-  <threadedComment ref="C47" dT="2019-12-31T16:35:39.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{B5C3BFB3-019D-426D-A008-79A436013E7A}">
+  <threadedComment ref="C45" dT="2019-12-31T16:35:39.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{B5C3BFB3-019D-426D-A008-79A436013E7A}">
     <text>0.27 m³/month @ G1360. Considering 18000 m², the average per m² is 0.000015</text>
   </threadedComment>
-  <threadedComment ref="C54" dT="2019-12-31T14:30:36.25" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{56892021-C2EB-47AE-B836-157999D31257}">
+  <threadedComment ref="C52" dT="2019-12-31T14:30:36.25" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{56892021-C2EB-47AE-B836-157999D31257}">
     <text>rome fiumicino</text>
   </threadedComment>
-  <threadedComment ref="C55" dT="2019-12-31T14:30:40.64" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{8A1481D7-3873-420A-9E14-35507B0A9525}">
+  <threadedComment ref="C53" dT="2019-12-31T14:30:40.64" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{8A1481D7-3873-420A-9E14-35507B0A9525}">
+    <text>rome fiumicino</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C18" dT="2019-12-31T13:50:55.89" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{396ABCAF-54DB-4DB8-9877-C4D9CB0C752F}">
+    <text>107087 kWh/month @ G1170. Considering 500 workers in the building, the average per worker is 214.17.</text>
+  </threadedComment>
+  <threadedComment ref="C19" dT="2019-12-31T14:01:21.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{DB4559B8-B4D5-46B8-9443-71ECDC1325D0}">
+    <text>190 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 0.38</text>
+  </threadedComment>
+  <threadedComment ref="C20" dT="2019-12-31T14:02:51.19" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{7E0439F0-61E6-4463-942E-D17301560662}">
+    <text>750 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 1.5</text>
+  </threadedComment>
+  <threadedComment ref="C44" dT="2019-12-31T14:53:25.54" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{0DC24375-CA62-42B8-82D8-58C5246FFD6F}">
+    <text>80000 kWh/month @ G1360. Considering 18000 m², the average per m² is 4.44</text>
+  </threadedComment>
+  <threadedComment ref="C45" dT="2019-12-31T14:55:29.34" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{72D2B639-7D47-4D27-A14C-D414C3B25E87}">
+    <text>80 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00444</text>
+  </threadedComment>
+  <threadedComment ref="C46" dT="2019-12-31T16:34:31.50" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{B1C3D0ED-7599-4C93-8848-AD9F3F4ACEF7}">
+    <text>64 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00356</text>
+  </threadedComment>
+  <threadedComment ref="C47" dT="2019-12-31T16:35:39.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{B5C3BFB3-019D-426E-A008-79A436013E7A}">
+    <text>0.27 m³/month @ G1360. Considering 18000 m², the average per m² is 0.000015</text>
+  </threadedComment>
+  <threadedComment ref="C54" dT="2019-12-31T14:30:36.25" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{56892021-C2EB-47AF-B836-157999D31257}">
+    <text>rome fiumicino</text>
+  </threadedComment>
+  <threadedComment ref="C55" dT="2019-12-31T14:30:40.64" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{8A1481D7-3873-420B-9E14-35507B0A9525}">
     <text>rome fiumicino</text>
   </threadedComment>
 </ThreadedComments>
@@ -1738,20 +1608,20 @@
   <dimension ref="A1:L122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="A11:XFD11"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.08984375" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.21875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="58" t="s">
         <v>4</v>
       </c>
@@ -1761,7 +1631,7 @@
       <c r="F1" s="59"/>
       <c r="G1" s="59"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="11"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1769,7 +1639,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1789,7 +1659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="60" t="s">
         <v>63</v>
       </c>
@@ -1801,12 +1671,12 @@
         <v>2.5</v>
       </c>
       <c r="D4" s="17">
-        <f>C4*0.8</f>
-        <v>2</v>
+        <f>C4</f>
+        <v>2.5</v>
       </c>
       <c r="E4" s="17">
-        <f>C4*1.2</f>
-        <v>3</v>
+        <f>C4</f>
+        <v>2.5</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>40</v>
@@ -1815,7 +1685,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="61"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
@@ -1824,12 +1694,12 @@
         <v>41244</v>
       </c>
       <c r="D5" s="46">
-        <f>C5*0.95</f>
-        <v>39181.799999999996</v>
+        <f t="shared" ref="D5:D68" si="0">C5</f>
+        <v>41244</v>
       </c>
       <c r="E5" s="46">
-        <f>C5*1.05</f>
-        <v>43306.200000000004</v>
+        <f t="shared" ref="E5:E68" si="1">C5</f>
+        <v>41244</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>8</v>
@@ -1838,7 +1708,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="61"/>
       <c r="B6" s="12" t="s">
         <v>52</v>
@@ -1847,10 +1717,11 @@
         <v>1920</v>
       </c>
       <c r="D6" s="17">
-        <f>C6*0.8</f>
-        <v>1536</v>
+        <f t="shared" si="0"/>
+        <v>1920</v>
       </c>
       <c r="E6" s="17">
+        <f t="shared" si="1"/>
         <v>1920</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1860,7 +1731,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="61"/>
       <c r="B7" s="12" t="s">
         <v>55</v>
@@ -1869,12 +1740,12 @@
         <v>1.82</v>
       </c>
       <c r="D7" s="17">
-        <f>C7*0.7</f>
-        <v>1.274</v>
+        <f t="shared" si="0"/>
+        <v>1.82</v>
       </c>
       <c r="E7" s="17">
-        <f>C7*1.1</f>
-        <v>2.0020000000000002</v>
+        <f t="shared" si="1"/>
+        <v>1.82</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>12</v>
@@ -1883,7 +1754,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="61"/>
       <c r="B8" s="12" t="s">
         <v>123</v>
@@ -1892,12 +1763,12 @@
         <v>180</v>
       </c>
       <c r="D8" s="17">
-        <f>C8*0.8</f>
-        <v>144</v>
+        <f t="shared" si="0"/>
+        <v>180</v>
       </c>
       <c r="E8" s="17">
-        <f>C8*1.1</f>
-        <v>198.00000000000003</v>
+        <f t="shared" si="1"/>
+        <v>180</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>6</v>
@@ -1906,7 +1777,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="61"/>
       <c r="B9" s="12" t="s">
         <v>5</v>
@@ -1915,18 +1786,19 @@
         <v>0.84</v>
       </c>
       <c r="D9" s="17">
-        <f>C9*0.8</f>
-        <v>0.67200000000000004</v>
+        <f t="shared" si="0"/>
+        <v>0.84</v>
       </c>
       <c r="E9" s="17">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.84</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="61"/>
       <c r="B10" s="12" t="s">
         <v>134</v>
@@ -1935,19 +1807,19 @@
         <v>0.78</v>
       </c>
       <c r="D10" s="17">
-        <f>C10*0.8</f>
-        <v>0.62400000000000011</v>
+        <f t="shared" si="0"/>
+        <v>0.78</v>
       </c>
       <c r="E10" s="17">
-        <f>C10*1.2</f>
-        <v>0.93599999999999994</v>
+        <f t="shared" si="1"/>
+        <v>0.78</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="61"/>
       <c r="B11" s="12" t="s">
         <v>7</v>
@@ -1956,12 +1828,12 @@
         <v>1100</v>
       </c>
       <c r="D11" s="17">
-        <f>C11*0.8</f>
-        <v>880</v>
+        <f t="shared" si="0"/>
+        <v>1100</v>
       </c>
       <c r="E11" s="17">
-        <f>C11*1.2</f>
-        <v>1320</v>
+        <f t="shared" si="1"/>
+        <v>1100</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>11</v>
@@ -1970,7 +1842,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="61"/>
       <c r="B12" s="12" t="s">
         <v>85</v>
@@ -1979,12 +1851,12 @@
         <v>25</v>
       </c>
       <c r="D12" s="17">
-        <f>C12*0.8</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="E12" s="17">
-        <f>C12*1.2</f>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>14</v>
@@ -1993,7 +1865,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="61"/>
       <c r="B13" s="12" t="s">
         <v>86</v>
@@ -2002,12 +1874,12 @@
         <v>4770</v>
       </c>
       <c r="D13" s="17">
-        <f>C13</f>
+        <f t="shared" si="0"/>
         <v>4770</v>
       </c>
       <c r="E13" s="17">
-        <f>C13*1.4</f>
-        <v>6678</v>
+        <f t="shared" si="1"/>
+        <v>4770</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>10</v>
@@ -2016,7 +1888,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
       <c r="B14" s="12" t="s">
         <v>34</v>
@@ -2025,19 +1897,19 @@
         <v>30</v>
       </c>
       <c r="D14" s="17">
-        <f>C14*0.8</f>
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="E14" s="17">
-        <f>C14*1.2</f>
-        <v>36</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="41"/>
       <c r="B15" s="12" t="s">
         <v>35</v>
@@ -2046,19 +1918,19 @@
         <v>60</v>
       </c>
       <c r="D15" s="17">
-        <f t="shared" ref="D15:D16" si="0">C15*0.8</f>
-        <v>48</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="E15" s="17">
-        <f t="shared" ref="E15:E16" si="1">C15*1.2</f>
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>60</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="12" t="s">
         <v>36</v>
@@ -2068,18 +1940,18 @@
       </c>
       <c r="D16" s="17">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E16" s="17">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="62" t="s">
         <v>88</v>
       </c>
@@ -2091,12 +1963,12 @@
         <v>42834.8</v>
       </c>
       <c r="D17" s="18">
-        <f>107087/500*D22</f>
-        <v>34267.840000000004</v>
+        <f t="shared" si="0"/>
+        <v>42834.8</v>
       </c>
       <c r="E17" s="18">
-        <f>107087/500*E22</f>
-        <v>51401.760000000002</v>
+        <f t="shared" si="1"/>
+        <v>42834.8</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>87</v>
@@ -2105,7 +1977,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="63"/>
       <c r="B18" s="13" t="s">
         <v>94</v>
@@ -2115,12 +1987,12 @@
         <v>76</v>
       </c>
       <c r="D18" s="18">
-        <f t="shared" ref="D18:E18" si="2">190/500*D22</f>
-        <v>60.8</v>
+        <f t="shared" si="0"/>
+        <v>76</v>
       </c>
       <c r="E18" s="18">
-        <f t="shared" si="2"/>
-        <v>91.2</v>
+        <f t="shared" si="1"/>
+        <v>76</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>105</v>
@@ -2129,7 +2001,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="63"/>
       <c r="B19" s="13" t="s">
         <v>95</v>
@@ -2139,12 +2011,12 @@
         <v>300</v>
       </c>
       <c r="D19" s="18">
-        <f t="shared" ref="D19:E19" si="3">3000/4/500*D22</f>
-        <v>240</v>
+        <f t="shared" si="0"/>
+        <v>300</v>
       </c>
       <c r="E19" s="18">
-        <f t="shared" si="3"/>
-        <v>360</v>
+        <f t="shared" si="1"/>
+        <v>300</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>105</v>
@@ -2153,7 +2025,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="42"/>
       <c r="B20" s="13" t="s">
         <v>124</v>
@@ -2162,12 +2034,12 @@
         <v>466</v>
       </c>
       <c r="D20" s="18">
-        <f>C20*0.8</f>
-        <v>372.8</v>
+        <f t="shared" si="0"/>
+        <v>466</v>
       </c>
       <c r="E20" s="18">
-        <f>C20*1.2</f>
-        <v>559.19999999999993</v>
+        <f t="shared" si="1"/>
+        <v>466</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>147</v>
@@ -2176,7 +2048,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="64" t="s">
         <v>90</v>
       </c>
@@ -2187,11 +2059,12 @@
         <v>48</v>
       </c>
       <c r="D21" s="38">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="E21" s="38">
-        <f>C21*1.2</f>
-        <v>57.599999999999994</v>
+        <f t="shared" si="1"/>
+        <v>48</v>
       </c>
       <c r="F21" s="39" t="s">
         <v>93</v>
@@ -2200,7 +2073,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="64"/>
       <c r="B22" s="37" t="s">
         <v>96</v>
@@ -2209,12 +2082,12 @@
         <v>200</v>
       </c>
       <c r="D22" s="40">
-        <f>C22*0.8</f>
-        <v>160</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="E22" s="40">
-        <f>C22*1.2</f>
-        <v>240</v>
+        <f t="shared" si="1"/>
+        <v>200</v>
       </c>
       <c r="F22" s="39" t="s">
         <v>98</v>
@@ -2223,7 +2096,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="64"/>
       <c r="B23" s="37" t="s">
         <v>106</v>
@@ -2233,11 +2106,11 @@
         <v>1539.1666666666667</v>
       </c>
       <c r="D23" s="40">
-        <f>C23</f>
+        <f t="shared" si="0"/>
         <v>1539.1666666666667</v>
       </c>
       <c r="E23" s="40">
-        <f>C23</f>
+        <f t="shared" si="1"/>
         <v>1539.1666666666667</v>
       </c>
       <c r="F23" s="39" t="s">
@@ -2247,7 +2120,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="64"/>
       <c r="B24" s="37" t="s">
         <v>109</v>
@@ -2257,11 +2130,11 @@
         <v>20000</v>
       </c>
       <c r="D24" s="40">
-        <f>C24</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="E24" s="40">
-        <f>C24</f>
+        <f t="shared" si="1"/>
         <v>20000</v>
       </c>
       <c r="F24" s="39" t="s">
@@ -2271,7 +2144,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="64"/>
       <c r="B25" s="37" t="s">
         <v>99</v>
@@ -2281,12 +2154,12 @@
         <v>19062</v>
       </c>
       <c r="D25" s="40">
-        <f>C25*0.6</f>
-        <v>11437.199999999999</v>
+        <f t="shared" si="0"/>
+        <v>19062</v>
       </c>
       <c r="E25" s="40">
-        <f>C25*1.4</f>
-        <v>26686.799999999999</v>
+        <f t="shared" si="1"/>
+        <v>19062</v>
       </c>
       <c r="F25" s="39" t="s">
         <v>103</v>
@@ -2295,7 +2168,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="64"/>
       <c r="B26" s="37" t="s">
         <v>100</v>
@@ -2304,12 +2177,12 @@
         <v>10</v>
       </c>
       <c r="D26" s="40">
-        <f>C26*0.4</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="E26" s="40">
-        <f>C26*1.6</f>
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="F26" s="39" t="s">
         <v>104</v>
@@ -2318,7 +2191,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="64"/>
       <c r="B27" s="37" t="s">
         <v>112</v>
@@ -2327,11 +2200,11 @@
         <v>5</v>
       </c>
       <c r="D27" s="40">
-        <f>C27</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E27" s="40">
-        <f>C27</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F27" s="39" t="s">
@@ -2341,7 +2214,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="64"/>
       <c r="B28" s="37" t="s">
         <v>113</v>
@@ -2350,11 +2223,11 @@
         <v>2</v>
       </c>
       <c r="D28" s="40">
-        <f>C28</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E28" s="40">
-        <f>C28</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F28" s="39" t="s">
@@ -2364,7 +2237,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="64"/>
       <c r="B29" s="37" t="s">
         <v>116</v>
@@ -2373,12 +2246,12 @@
         <v>3100</v>
       </c>
       <c r="D29" s="40">
-        <f>C29*0.8</f>
-        <v>2480</v>
+        <f t="shared" si="0"/>
+        <v>3100</v>
       </c>
       <c r="E29" s="40">
-        <f>C29*1.2</f>
-        <v>3720</v>
+        <f t="shared" si="1"/>
+        <v>3100</v>
       </c>
       <c r="F29" s="39" t="s">
         <v>12</v>
@@ -2387,7 +2260,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="65" t="s">
         <v>60</v>
       </c>
@@ -2395,171 +2268,169 @@
         <v>21</v>
       </c>
       <c r="C30" s="19">
-        <v>0.46</v>
+        <v>1</v>
       </c>
       <c r="D30" s="19">
-        <f>C30*0.8</f>
-        <v>0.36800000000000005</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E30" s="19">
-        <f>C30*1.2</f>
-        <v>0.55200000000000005</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="66"/>
       <c r="B31" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="19">
-        <v>0.7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D31" s="19">
-        <f t="shared" ref="D31:D41" si="4">C31*0.8</f>
-        <v>0.55999999999999994</v>
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E31" s="19">
-        <f t="shared" ref="E31:E41" si="5">C31*1.2</f>
-        <v>0.84</v>
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="66"/>
       <c r="B32" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="19">
-        <f>0.32/2</f>
-        <v>0.16</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D32" s="19">
-        <f t="shared" si="4"/>
-        <v>0.128</v>
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E32" s="19">
-        <f t="shared" si="5"/>
-        <v>0.192</v>
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="66"/>
       <c r="B33" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="19">
-        <f>C32</f>
-        <v>0.16</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D33" s="19">
-        <f t="shared" si="4"/>
-        <v>0.128</v>
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E33" s="19">
-        <f t="shared" si="5"/>
-        <v>0.192</v>
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="66"/>
       <c r="B34" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="19">
-        <v>0.05</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D34" s="19">
-        <f t="shared" si="4"/>
-        <v>4.0000000000000008E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E34" s="19">
-        <f t="shared" si="5"/>
-        <v>0.06</v>
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="66"/>
       <c r="B35" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="19">
-        <v>0.1</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D35" s="19">
-        <f t="shared" si="4"/>
-        <v>8.0000000000000016E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E35" s="19">
-        <f t="shared" si="5"/>
-        <v>0.12</v>
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="66"/>
       <c r="B36" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="19">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D36" s="19">
-        <f t="shared" si="4"/>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="E36" s="19">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="66"/>
       <c r="B37" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="19">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D37" s="19">
-        <f t="shared" si="4"/>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="E37" s="19">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="66"/>
       <c r="B38" s="14" t="s">
         <v>28</v>
@@ -2568,19 +2439,19 @@
         <v>1.2</v>
       </c>
       <c r="D38" s="19">
-        <f t="shared" si="4"/>
-        <v>0.96</v>
+        <f t="shared" si="0"/>
+        <v>1.2</v>
       </c>
       <c r="E38" s="19">
-        <f t="shared" si="5"/>
-        <v>1.44</v>
+        <f t="shared" si="1"/>
+        <v>1.2</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="66"/>
       <c r="B39" s="14" t="s">
         <v>32</v>
@@ -2589,61 +2460,61 @@
         <v>1.2</v>
       </c>
       <c r="D39" s="19">
-        <f t="shared" si="4"/>
-        <v>0.96</v>
+        <f t="shared" si="0"/>
+        <v>1.2</v>
       </c>
       <c r="E39" s="19">
-        <f t="shared" si="5"/>
-        <v>1.44</v>
+        <f t="shared" si="1"/>
+        <v>1.2</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="66"/>
       <c r="B40" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C40" s="19">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D40" s="19">
-        <f t="shared" si="4"/>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="E40" s="19">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="66"/>
       <c r="B41" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="19">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D41" s="19">
-        <f t="shared" si="4"/>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="E41" s="19">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="67" t="s">
         <v>61</v>
       </c>
@@ -2655,12 +2526,12 @@
         <v>169440</v>
       </c>
       <c r="D42" s="23">
-        <f>C42*0.8</f>
-        <v>135552</v>
+        <f t="shared" si="0"/>
+        <v>169440</v>
       </c>
       <c r="E42" s="23">
-        <f>C42*1.2</f>
-        <v>203328</v>
+        <f t="shared" si="1"/>
+        <v>169440</v>
       </c>
       <c r="F42" s="24" t="s">
         <v>87</v>
@@ -2669,7 +2540,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="68"/>
       <c r="B43" s="22" t="s">
         <v>37</v>
@@ -2679,12 +2550,12 @@
         <v>169.44</v>
       </c>
       <c r="D43" s="23">
-        <f t="shared" ref="D43:D45" si="6">C43*0.8</f>
-        <v>135.55199999999999</v>
+        <f t="shared" si="0"/>
+        <v>169.44</v>
       </c>
       <c r="E43" s="23">
-        <f t="shared" ref="E43:E45" si="7">C43*1.2</f>
-        <v>203.328</v>
+        <f t="shared" si="1"/>
+        <v>169.44</v>
       </c>
       <c r="F43" s="24" t="s">
         <v>105</v>
@@ -2693,7 +2564,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="68"/>
       <c r="B44" s="22" t="s">
         <v>38</v>
@@ -2703,12 +2574,12 @@
         <v>135.55199999999999</v>
       </c>
       <c r="D44" s="23">
-        <f t="shared" si="6"/>
-        <v>108.44159999999999</v>
+        <f t="shared" si="0"/>
+        <v>135.55199999999999</v>
       </c>
       <c r="E44" s="23">
-        <f t="shared" si="7"/>
-        <v>162.66239999999999</v>
+        <f t="shared" si="1"/>
+        <v>135.55199999999999</v>
       </c>
       <c r="F44" s="24" t="s">
         <v>105</v>
@@ -2717,7 +2588,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="69"/>
       <c r="B45" s="22" t="s">
         <v>39</v>
@@ -2727,12 +2598,12 @@
         <v>0.56762400000000002</v>
       </c>
       <c r="D45" s="23">
-        <f t="shared" si="6"/>
-        <v>0.45409920000000004</v>
+        <f t="shared" si="0"/>
+        <v>0.56762400000000002</v>
       </c>
       <c r="E45" s="23">
-        <f t="shared" si="7"/>
-        <v>0.6811488</v>
+        <f t="shared" si="1"/>
+        <v>0.56762400000000002</v>
       </c>
       <c r="F45" s="24" t="s">
         <v>105</v>
@@ -2741,7 +2612,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="52" t="s">
         <v>62</v>
       </c>
@@ -2752,12 +2623,12 @@
         <v>1500</v>
       </c>
       <c r="D46" s="26">
-        <f>C46*0.8</f>
-        <v>1200</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="E46" s="26">
-        <f>C46*1.2</f>
-        <v>1800</v>
+        <f t="shared" si="1"/>
+        <v>1500</v>
       </c>
       <c r="F46" s="27" t="s">
         <v>11</v>
@@ -2766,7 +2637,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="52"/>
       <c r="B47" s="25" t="s">
         <v>43</v>
@@ -2775,12 +2646,12 @@
         <v>2000</v>
       </c>
       <c r="D47" s="26">
-        <f t="shared" ref="D47:D51" si="8">C47*0.8</f>
-        <v>1600</v>
+        <f t="shared" si="0"/>
+        <v>2000</v>
       </c>
       <c r="E47" s="26">
-        <f t="shared" ref="E47:E51" si="9">C47*1.2</f>
-        <v>2400</v>
+        <f t="shared" si="1"/>
+        <v>2000</v>
       </c>
       <c r="F47" s="27" t="s">
         <v>11</v>
@@ -2789,7 +2660,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="52"/>
       <c r="B48" s="25" t="s">
         <v>44</v>
@@ -2798,12 +2669,12 @@
         <v>500</v>
       </c>
       <c r="D48" s="26">
-        <f t="shared" si="8"/>
-        <v>400</v>
+        <f t="shared" si="0"/>
+        <v>500</v>
       </c>
       <c r="E48" s="26">
-        <f t="shared" si="9"/>
-        <v>600</v>
+        <f t="shared" si="1"/>
+        <v>500</v>
       </c>
       <c r="F48" s="27" t="s">
         <v>11</v>
@@ -2812,7 +2683,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="52"/>
       <c r="B49" s="25" t="s">
         <v>45</v>
@@ -2821,12 +2692,12 @@
         <v>20</v>
       </c>
       <c r="D49" s="26">
-        <f t="shared" si="8"/>
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="E49" s="26">
-        <f t="shared" si="9"/>
-        <v>24</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="F49" s="27" t="s">
         <v>48</v>
@@ -2835,7 +2706,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="52"/>
       <c r="B50" s="25" t="s">
         <v>46</v>
@@ -2844,12 +2715,12 @@
         <v>20</v>
       </c>
       <c r="D50" s="26">
-        <f t="shared" si="8"/>
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="E50" s="26">
-        <f t="shared" si="9"/>
-        <v>24</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="F50" s="27" t="s">
         <v>48</v>
@@ -2858,7 +2729,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="52"/>
       <c r="B51" s="25" t="s">
         <v>47</v>
@@ -2867,12 +2738,12 @@
         <v>1</v>
       </c>
       <c r="D51" s="26">
-        <f t="shared" si="8"/>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E51" s="26">
-        <f t="shared" si="9"/>
-        <v>1.2</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="F51" s="27" t="s">
         <v>48</v>
@@ -2881,7 +2752,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="53" t="s">
         <v>125</v>
       </c>
@@ -2892,12 +2763,12 @@
         <v>48800000</v>
       </c>
       <c r="D52" s="20">
-        <f t="shared" ref="D52:D53" si="10">C52</f>
+        <f t="shared" si="0"/>
         <v>48800000</v>
       </c>
       <c r="E52" s="20">
-        <f>C52*1.1</f>
-        <v>53680000.000000007</v>
+        <f t="shared" si="1"/>
+        <v>48800000</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>51</v>
@@ -2906,7 +2777,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="53"/>
       <c r="B53" s="15" t="s">
         <v>53</v>
@@ -2915,12 +2786,12 @@
         <v>307736</v>
       </c>
       <c r="D53" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>307736</v>
       </c>
       <c r="E53" s="20">
-        <f>C53*1.1</f>
-        <v>338509.60000000003</v>
+        <f t="shared" si="1"/>
+        <v>307736</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>13</v>
@@ -2929,7 +2800,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="54" t="s">
         <v>59</v>
       </c>
@@ -2941,12 +2812,12 @@
         <v>0.47222222222222221</v>
       </c>
       <c r="D54" s="43">
-        <f>C54*0.8</f>
-        <v>0.37777777777777777</v>
+        <f t="shared" si="0"/>
+        <v>0.47222222222222221</v>
       </c>
       <c r="E54" s="43">
-        <f>C54*1.2</f>
-        <v>0.56666666666666665</v>
+        <f t="shared" si="1"/>
+        <v>0.47222222222222221</v>
       </c>
       <c r="F54" s="30" t="s">
         <v>20</v>
@@ -2956,7 +2827,7 @@
       </c>
       <c r="L54" s="21"/>
     </row>
-    <row r="55" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="55"/>
       <c r="B55" s="28" t="s">
         <v>56</v>
@@ -2966,12 +2837,12 @@
         <v>4.54</v>
       </c>
       <c r="D55" s="29">
-        <f t="shared" ref="D55:D66" si="11">C55*0.8</f>
-        <v>3.6320000000000001</v>
+        <f t="shared" si="0"/>
+        <v>4.54</v>
       </c>
       <c r="E55" s="29">
-        <f t="shared" ref="E55:E66" si="12">C55*1.2</f>
-        <v>5.4479999999999995</v>
+        <f t="shared" si="1"/>
+        <v>4.54</v>
       </c>
       <c r="F55" s="30" t="s">
         <v>58</v>
@@ -2981,7 +2852,7 @@
       </c>
       <c r="L55" s="21"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="55"/>
       <c r="B56" s="28" t="s">
         <v>57</v>
@@ -2991,12 +2862,12 @@
         <v>44</v>
       </c>
       <c r="D56" s="29">
-        <f t="shared" si="11"/>
-        <v>35.200000000000003</v>
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="E56" s="29">
-        <f t="shared" si="12"/>
-        <v>52.8</v>
+        <f t="shared" si="1"/>
+        <v>44</v>
       </c>
       <c r="F56" s="30" t="s">
         <v>58</v>
@@ -3006,7 +2877,7 @@
       </c>
       <c r="L56" s="21"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="55"/>
       <c r="B57" s="28" t="s">
         <v>118</v>
@@ -3016,12 +2887,12 @@
         <v>0.9</v>
       </c>
       <c r="D57" s="29">
-        <f t="shared" si="11"/>
-        <v>0.72000000000000008</v>
+        <f t="shared" si="0"/>
+        <v>0.9</v>
       </c>
       <c r="E57" s="29">
-        <f t="shared" si="12"/>
-        <v>1.08</v>
+        <f t="shared" si="1"/>
+        <v>0.9</v>
       </c>
       <c r="F57" s="30" t="s">
         <v>58</v>
@@ -3031,7 +2902,7 @@
       </c>
       <c r="L57" s="21"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="55"/>
       <c r="B58" s="28" t="s">
         <v>119</v>
@@ -3041,12 +2912,12 @@
         <v>10.665600000000001</v>
       </c>
       <c r="D58" s="29">
-        <f t="shared" si="11"/>
-        <v>8.5324800000000014</v>
+        <f t="shared" si="0"/>
+        <v>10.665600000000001</v>
       </c>
       <c r="E58" s="29">
-        <f t="shared" si="12"/>
-        <v>12.798720000000001</v>
+        <f t="shared" si="1"/>
+        <v>10.665600000000001</v>
       </c>
       <c r="F58" s="30" t="s">
         <v>58</v>
@@ -3056,7 +2927,7 @@
       </c>
       <c r="L58" s="21"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="55"/>
       <c r="B59" s="28" t="s">
         <v>64</v>
@@ -3065,12 +2936,12 @@
         <v>4</v>
       </c>
       <c r="D59" s="29">
-        <f t="shared" si="11"/>
-        <v>3.2</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E59" s="29">
-        <f t="shared" si="12"/>
-        <v>4.8</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="F59" s="30" t="s">
         <v>19</v>
@@ -3080,7 +2951,7 @@
       </c>
       <c r="L59" s="21"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="55"/>
       <c r="B60" s="28" t="s">
         <v>65</v>
@@ -3089,12 +2960,12 @@
         <v>26</v>
       </c>
       <c r="D60" s="29">
-        <f t="shared" si="11"/>
-        <v>20.8</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="E60" s="29">
-        <f t="shared" si="12"/>
-        <v>31.2</v>
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
       <c r="F60" s="30" t="s">
         <v>19</v>
@@ -3104,7 +2975,7 @@
       </c>
       <c r="L60" s="21"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="55"/>
       <c r="B61" s="28" t="s">
         <v>66</v>
@@ -3113,12 +2984,12 @@
         <v>0.7</v>
       </c>
       <c r="D61" s="29">
-        <f t="shared" si="11"/>
-        <v>0.55999999999999994</v>
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
       <c r="E61" s="29">
-        <f t="shared" si="12"/>
-        <v>0.84</v>
+        <f t="shared" si="1"/>
+        <v>0.7</v>
       </c>
       <c r="F61" s="30" t="s">
         <v>19</v>
@@ -3128,7 +2999,7 @@
       </c>
       <c r="L61" s="21"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="55"/>
       <c r="B62" s="28" t="s">
         <v>67</v>
@@ -3137,12 +3008,12 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D62" s="29">
-        <f t="shared" si="11"/>
-        <v>1.7600000000000002</v>
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E62" s="29">
-        <f t="shared" si="12"/>
-        <v>2.64</v>
+        <f t="shared" si="1"/>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F62" s="30" t="s">
         <v>19</v>
@@ -3152,7 +3023,7 @@
       </c>
       <c r="L62" s="21"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="55"/>
       <c r="B63" s="28" t="s">
         <v>15</v>
@@ -3161,12 +3032,12 @@
         <v>0.27600000000000002</v>
       </c>
       <c r="D63" s="29">
-        <f t="shared" si="11"/>
-        <v>0.22080000000000002</v>
+        <f t="shared" si="0"/>
+        <v>0.27600000000000002</v>
       </c>
       <c r="E63" s="29">
-        <f t="shared" si="12"/>
-        <v>0.33119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.27600000000000002</v>
       </c>
       <c r="F63" s="30" t="s">
         <v>20</v>
@@ -3176,7 +3047,7 @@
       </c>
       <c r="L63" s="21"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="55"/>
       <c r="B64" s="28" t="s">
         <v>16</v>
@@ -3185,12 +3056,12 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="D64" s="29">
-        <f t="shared" si="11"/>
-        <v>7.6800000000000007E-2</v>
+        <f t="shared" si="0"/>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="E64" s="29">
-        <f t="shared" si="12"/>
-        <v>0.1152</v>
+        <f t="shared" si="1"/>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="F64" s="30" t="s">
         <v>20</v>
@@ -3200,7 +3071,7 @@
       </c>
       <c r="L64" s="21"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="55"/>
       <c r="B65" s="28" t="s">
         <v>17</v>
@@ -3209,12 +3080,12 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="D65" s="29">
-        <f t="shared" si="11"/>
-        <v>0.77760000000000007</v>
+        <f t="shared" si="0"/>
+        <v>0.97199999999999998</v>
       </c>
       <c r="E65" s="29">
-        <f t="shared" si="12"/>
-        <v>1.1663999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.97199999999999998</v>
       </c>
       <c r="F65" s="30" t="s">
         <v>20</v>
@@ -3223,7 +3094,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="55"/>
       <c r="B66" s="35" t="s">
         <v>18</v>
@@ -3232,12 +3103,12 @@
         <v>0.79900000000000004</v>
       </c>
       <c r="D66" s="29">
-        <f t="shared" si="11"/>
-        <v>0.6392000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.79900000000000004</v>
       </c>
       <c r="E66" s="29">
-        <f t="shared" si="12"/>
-        <v>0.95879999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.79900000000000004</v>
       </c>
       <c r="F66" s="36" t="s">
         <v>20</v>
@@ -3247,7 +3118,7 @@
       </c>
       <c r="L66" s="21"/>
     </row>
-    <row r="67" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="56" t="s">
         <v>69</v>
       </c>
@@ -3258,11 +3129,11 @@
         <v>0.25</v>
       </c>
       <c r="D67" s="32">
-        <f>C67</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="E67" s="32">
-        <f>C67</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F67" s="33"/>
@@ -3270,7 +3141,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="57"/>
       <c r="B68" s="31" t="s">
         <v>79</v>
@@ -3279,11 +3150,11 @@
         <v>0.2</v>
       </c>
       <c r="D68" s="32">
-        <f t="shared" ref="D68:D84" si="13">C68</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="E68" s="32">
-        <f t="shared" ref="E68:E84" si="14">C68</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F68" s="33"/>
@@ -3291,7 +3162,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="57"/>
       <c r="B69" s="31" t="s">
         <v>71</v>
@@ -3300,11 +3171,11 @@
         <v>0.2</v>
       </c>
       <c r="D69" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="D69:D84" si="2">C69</f>
         <v>0.2</v>
       </c>
       <c r="E69" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="E69:E84" si="3">C69</f>
         <v>0.2</v>
       </c>
       <c r="F69" s="33"/>
@@ -3312,7 +3183,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="57"/>
       <c r="B70" s="31" t="s">
         <v>72</v>
@@ -3321,11 +3192,11 @@
         <v>0.2</v>
       </c>
       <c r="D70" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="E70" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="F70" s="33"/>
@@ -3333,7 +3204,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="57"/>
       <c r="B71" s="31" t="s">
         <v>73</v>
@@ -3342,11 +3213,11 @@
         <v>0.5</v>
       </c>
       <c r="D71" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E71" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="F71" s="33"/>
@@ -3354,7 +3225,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="57"/>
       <c r="B72" s="31" t="s">
         <v>120</v>
@@ -3363,11 +3234,11 @@
         <v>0.5</v>
       </c>
       <c r="D72" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E72" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="F72" s="33"/>
@@ -3375,7 +3246,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="57"/>
       <c r="B73" s="31" t="s">
         <v>74</v>
@@ -3384,11 +3255,11 @@
         <v>0.25</v>
       </c>
       <c r="D73" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="E73" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="F73" s="33"/>
@@ -3397,7 +3268,7 @@
       </c>
       <c r="L73" s="21"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="57"/>
       <c r="B74" s="31" t="s">
         <v>80</v>
@@ -3406,11 +3277,11 @@
         <v>0.1</v>
       </c>
       <c r="D74" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="E74" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="F74" s="33"/>
@@ -3419,7 +3290,7 @@
       </c>
       <c r="L74" s="21"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="57"/>
       <c r="B75" s="31" t="s">
         <v>75</v>
@@ -3428,11 +3299,11 @@
         <v>0.1</v>
       </c>
       <c r="D75" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="E75" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="F75" s="33"/>
@@ -3441,7 +3312,7 @@
       </c>
       <c r="L75" s="21"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="57"/>
       <c r="B76" s="31" t="s">
         <v>76</v>
@@ -3450,11 +3321,11 @@
         <v>0.1</v>
       </c>
       <c r="D76" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="E76" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="F76" s="33"/>
@@ -3463,7 +3334,7 @@
       </c>
       <c r="L76" s="21"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="57"/>
       <c r="B77" s="31" t="s">
         <v>77</v>
@@ -3472,11 +3343,11 @@
         <v>0.45</v>
       </c>
       <c r="D77" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.45</v>
       </c>
       <c r="E77" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.45</v>
       </c>
       <c r="F77" s="33"/>
@@ -3485,7 +3356,7 @@
       </c>
       <c r="L77" s="21"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="57"/>
       <c r="B78" s="31" t="s">
         <v>122</v>
@@ -3494,11 +3365,11 @@
         <v>0.45</v>
       </c>
       <c r="D78" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.45</v>
       </c>
       <c r="E78" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.45</v>
       </c>
       <c r="F78" s="33"/>
@@ -3507,7 +3378,7 @@
       </c>
       <c r="L78" s="21"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="57"/>
       <c r="B79" s="31" t="s">
         <v>78</v>
@@ -3516,11 +3387,11 @@
         <v>0.5</v>
       </c>
       <c r="D79" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E79" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="F79" s="33"/>
@@ -3528,7 +3399,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="57"/>
       <c r="B80" s="31" t="s">
         <v>81</v>
@@ -3537,11 +3408,11 @@
         <v>0.7</v>
       </c>
       <c r="D80" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
       <c r="E80" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="F80" s="33"/>
@@ -3549,7 +3420,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="57"/>
       <c r="B81" s="31" t="s">
         <v>82</v>
@@ -3558,11 +3429,11 @@
         <v>0.7</v>
       </c>
       <c r="D81" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
       <c r="E81" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="F81" s="33"/>
@@ -3570,7 +3441,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="57"/>
       <c r="B82" s="31" t="s">
         <v>83</v>
@@ -3579,11 +3450,11 @@
         <v>0.7</v>
       </c>
       <c r="D82" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
       <c r="E82" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="F82" s="33"/>
@@ -3591,7 +3462,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="57"/>
       <c r="B83" s="31" t="s">
         <v>84</v>
@@ -3600,11 +3471,11 @@
         <v>0.05</v>
       </c>
       <c r="D83" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="E83" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="F83" s="33"/>
@@ -3612,7 +3483,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="57"/>
       <c r="B84" s="31" t="s">
         <v>121</v>
@@ -3621,11 +3492,11 @@
         <v>0.05</v>
       </c>
       <c r="D84" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="E84" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="F84" s="33"/>
@@ -3633,52 +3504,52 @@
         <v>207</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L86" s="21"/>
     </row>
-    <row r="104" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L104" s="21"/>
     </row>
-    <row r="108" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L108" s="21"/>
     </row>
-    <row r="109" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L109" s="21"/>
     </row>
-    <row r="110" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L110" s="21"/>
     </row>
-    <row r="111" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L111" s="21"/>
     </row>
-    <row r="112" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L112" s="21"/>
     </row>
-    <row r="113" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L113" s="21"/>
     </row>
-    <row r="114" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L114" s="21"/>
     </row>
-    <row r="115" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L115" s="21"/>
     </row>
-    <row r="116" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L116" s="21"/>
     </row>
-    <row r="117" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L117" s="21"/>
     </row>
-    <row r="118" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L118" s="21"/>
     </row>
-    <row r="119" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L119" s="21"/>
     </row>
-    <row r="120" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L120" s="21"/>
     </row>
-    <row r="122" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L122" s="21"/>
     </row>
   </sheetData>
@@ -3708,16 +3579,16 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.08984375" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.21875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="58" t="s">
         <v>4</v>
       </c>
@@ -3727,7 +3598,7 @@
       <c r="F1" s="59"/>
       <c r="G1" s="59"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="11"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -3735,7 +3606,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -3755,7 +3626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="60" t="s">
         <v>63</v>
       </c>
@@ -3781,7 +3652,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="61"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
@@ -3804,7 +3675,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="61"/>
       <c r="B6" s="12" t="s">
         <v>52</v>
@@ -3826,7 +3697,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="61"/>
       <c r="B7" s="12" t="s">
         <v>55</v>
@@ -3849,7 +3720,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="61"/>
       <c r="B8" s="12" t="s">
         <v>123</v>
@@ -3872,7 +3743,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="61"/>
       <c r="B9" s="12" t="s">
         <v>5</v>
@@ -3892,7 +3763,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="61"/>
       <c r="B10" s="12" t="s">
         <v>134</v>
@@ -3913,7 +3784,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="61"/>
       <c r="B11" s="12" t="s">
         <v>136</v>
@@ -3928,7 +3799,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="61"/>
       <c r="B12" s="12" t="s">
         <v>7</v>
@@ -3951,7 +3822,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="61"/>
       <c r="B13" s="12" t="s">
         <v>85</v>
@@ -3974,7 +3845,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="61"/>
       <c r="B14" s="12" t="s">
         <v>86</v>
@@ -3997,7 +3868,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="49"/>
       <c r="B15" s="12" t="s">
         <v>34</v>
@@ -4018,7 +3889,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="49"/>
       <c r="B16" s="12" t="s">
         <v>35</v>
@@ -4039,7 +3910,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="49"/>
       <c r="B17" s="12" t="s">
         <v>36</v>
@@ -4060,7 +3931,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="62" t="s">
         <v>88</v>
       </c>
@@ -4086,7 +3957,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="63"/>
       <c r="B19" s="13" t="s">
         <v>94</v>
@@ -4110,7 +3981,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="63"/>
       <c r="B20" s="13" t="s">
         <v>95</v>
@@ -4134,7 +4005,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="50"/>
       <c r="B21" s="13" t="s">
         <v>124</v>
@@ -4157,7 +4028,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="64" t="s">
         <v>90</v>
       </c>
@@ -4181,7 +4052,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="64"/>
       <c r="B23" s="37" t="s">
         <v>96</v>
@@ -4204,7 +4075,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="64"/>
       <c r="B24" s="37" t="s">
         <v>106</v>
@@ -4228,7 +4099,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="64"/>
       <c r="B25" s="37" t="s">
         <v>109</v>
@@ -4252,7 +4123,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="64"/>
       <c r="B26" s="37" t="s">
         <v>99</v>
@@ -4276,7 +4147,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="64"/>
       <c r="B27" s="37" t="s">
         <v>100</v>
@@ -4299,7 +4170,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="64"/>
       <c r="B28" s="37" t="s">
         <v>112</v>
@@ -4322,7 +4193,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="64"/>
       <c r="B29" s="37" t="s">
         <v>113</v>
@@ -4345,7 +4216,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="64"/>
       <c r="B30" s="37" t="s">
         <v>116</v>
@@ -4368,7 +4239,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="65" t="s">
         <v>60</v>
       </c>
@@ -4391,7 +4262,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="66"/>
       <c r="B32" s="14" t="s">
         <v>22</v>
@@ -4412,7 +4283,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="66"/>
       <c r="B33" s="14" t="s">
         <v>23</v>
@@ -4434,7 +4305,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="66"/>
       <c r="B34" s="14" t="s">
         <v>31</v>
@@ -4456,7 +4327,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="66"/>
       <c r="B35" s="14" t="s">
         <v>24</v>
@@ -4477,7 +4348,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="66"/>
       <c r="B36" s="14" t="s">
         <v>25</v>
@@ -4498,7 +4369,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="66"/>
       <c r="B37" s="14" t="s">
         <v>26</v>
@@ -4519,7 +4390,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="66"/>
       <c r="B38" s="14" t="s">
         <v>27</v>
@@ -4540,7 +4411,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="66"/>
       <c r="B39" s="14" t="s">
         <v>28</v>
@@ -4561,7 +4432,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="66"/>
       <c r="B40" s="14" t="s">
         <v>32</v>
@@ -4582,7 +4453,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="66"/>
       <c r="B41" s="14" t="s">
         <v>29</v>
@@ -4603,7 +4474,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="66"/>
       <c r="B42" s="14" t="s">
         <v>30</v>
@@ -4624,7 +4495,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="51"/>
       <c r="B43" s="14" t="s">
         <v>161</v>
@@ -4637,7 +4508,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="67" t="s">
         <v>61</v>
       </c>
@@ -4663,7 +4534,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="68"/>
       <c r="B45" s="22" t="s">
         <v>37</v>
@@ -4687,7 +4558,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="68"/>
       <c r="B46" s="22" t="s">
         <v>38</v>
@@ -4711,7 +4582,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="69"/>
       <c r="B47" s="22" t="s">
         <v>39</v>
@@ -4735,7 +4606,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="52" t="s">
         <v>62</v>
       </c>
@@ -4760,7 +4631,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="52"/>
       <c r="B49" s="25" t="s">
         <v>43</v>
@@ -4783,7 +4654,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="52"/>
       <c r="B50" s="25" t="s">
         <v>44</v>
@@ -4806,7 +4677,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="52"/>
       <c r="B51" s="25" t="s">
         <v>45</v>
@@ -4829,7 +4700,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="52"/>
       <c r="B52" s="25" t="s">
         <v>46</v>
@@ -4852,7 +4723,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="52"/>
       <c r="B53" s="25" t="s">
         <v>47</v>
@@ -4875,7 +4746,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="53" t="s">
         <v>125</v>
       </c>
@@ -4900,7 +4771,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="53"/>
       <c r="B55" s="15" t="s">
         <v>53</v>
@@ -4923,7 +4794,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="54" t="s">
         <v>59</v>
       </c>
@@ -4950,7 +4821,7 @@
       </c>
       <c r="L56" s="21"/>
     </row>
-    <row r="57" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="55"/>
       <c r="B57" s="28" t="s">
         <v>56</v>
@@ -4975,7 +4846,7 @@
       </c>
       <c r="L57" s="21"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="55"/>
       <c r="B58" s="28" t="s">
         <v>57</v>
@@ -5000,7 +4871,7 @@
       </c>
       <c r="L58" s="21"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="55"/>
       <c r="B59" s="28" t="s">
         <v>118</v>
@@ -5025,7 +4896,7 @@
       </c>
       <c r="L59" s="21"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="55"/>
       <c r="B60" s="28" t="s">
         <v>119</v>
@@ -5050,7 +4921,7 @@
       </c>
       <c r="L60" s="21"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="55"/>
       <c r="B61" s="28" t="s">
         <v>64</v>
@@ -5074,7 +4945,7 @@
       </c>
       <c r="L61" s="21"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="55"/>
       <c r="B62" s="28" t="s">
         <v>65</v>
@@ -5098,7 +4969,7 @@
       </c>
       <c r="L62" s="21"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="55"/>
       <c r="B63" s="28" t="s">
         <v>66</v>
@@ -5122,7 +4993,7 @@
       </c>
       <c r="L63" s="21"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="55"/>
       <c r="B64" s="28" t="s">
         <v>67</v>
@@ -5146,7 +5017,7 @@
       </c>
       <c r="L64" s="21"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="55"/>
       <c r="B65" s="28" t="s">
         <v>182</v>
@@ -5162,7 +5033,7 @@
       </c>
       <c r="L65" s="21"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="55"/>
       <c r="B66" s="28" t="s">
         <v>15</v>
@@ -5186,7 +5057,7 @@
       </c>
       <c r="L66" s="21"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="55"/>
       <c r="B67" s="28" t="s">
         <v>16</v>
@@ -5210,7 +5081,7 @@
       </c>
       <c r="L67" s="21"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="55"/>
       <c r="B68" s="28" t="s">
         <v>17</v>
@@ -5233,7 +5104,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="55"/>
       <c r="B69" s="35" t="s">
         <v>18</v>
@@ -5257,7 +5128,7 @@
       </c>
       <c r="L69" s="21"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="44"/>
       <c r="B70" s="35" t="s">
         <v>188</v>
@@ -5273,7 +5144,7 @@
       </c>
       <c r="L70" s="21"/>
     </row>
-    <row r="71" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="56" t="s">
         <v>69</v>
       </c>
@@ -5296,7 +5167,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="57"/>
       <c r="B72" s="31" t="s">
         <v>79</v>
@@ -5317,7 +5188,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="57"/>
       <c r="B73" s="31" t="s">
         <v>71</v>
@@ -5338,7 +5209,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="57"/>
       <c r="B74" s="31" t="s">
         <v>72</v>
@@ -5359,7 +5230,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="57"/>
       <c r="B75" s="31" t="s">
         <v>73</v>
@@ -5380,7 +5251,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="57"/>
       <c r="B76" s="31" t="s">
         <v>120</v>
@@ -5401,7 +5272,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="57"/>
       <c r="B77" s="31" t="s">
         <v>74</v>
@@ -5423,7 +5294,7 @@
       </c>
       <c r="L77" s="21"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="57"/>
       <c r="B78" s="31" t="s">
         <v>80</v>
@@ -5445,7 +5316,7 @@
       </c>
       <c r="L78" s="21"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="57"/>
       <c r="B79" s="31" t="s">
         <v>75</v>
@@ -5467,7 +5338,7 @@
       </c>
       <c r="L79" s="21"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="57"/>
       <c r="B80" s="31" t="s">
         <v>76</v>
@@ -5489,7 +5360,7 @@
       </c>
       <c r="L80" s="21"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="57"/>
       <c r="B81" s="31" t="s">
         <v>77</v>
@@ -5511,7 +5382,7 @@
       </c>
       <c r="L81" s="21"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="57"/>
       <c r="B82" s="31" t="s">
         <v>122</v>
@@ -5533,7 +5404,7 @@
       </c>
       <c r="L82" s="21"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="57"/>
       <c r="B83" s="31" t="s">
         <v>78</v>
@@ -5554,7 +5425,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="57"/>
       <c r="B84" s="31" t="s">
         <v>81</v>
@@ -5575,7 +5446,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="57"/>
       <c r="B85" s="31" t="s">
         <v>82</v>
@@ -5596,7 +5467,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="57"/>
       <c r="B86" s="31" t="s">
         <v>83</v>
@@ -5617,7 +5488,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="57"/>
       <c r="B87" s="31" t="s">
         <v>84</v>
@@ -5638,7 +5509,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="57"/>
       <c r="B88" s="31" t="s">
         <v>121</v>
@@ -5659,52 +5530,52 @@
         <v>207</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L90" s="21"/>
     </row>
-    <row r="108" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L108" s="21"/>
     </row>
-    <row r="112" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L112" s="21"/>
     </row>
-    <row r="113" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L113" s="21"/>
     </row>
-    <row r="114" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L114" s="21"/>
     </row>
-    <row r="115" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L115" s="21"/>
     </row>
-    <row r="116" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L116" s="21"/>
     </row>
-    <row r="117" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L117" s="21"/>
     </row>
-    <row r="118" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L118" s="21"/>
     </row>
-    <row r="119" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L119" s="21"/>
     </row>
-    <row r="120" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L120" s="21"/>
     </row>
-    <row r="121" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L121" s="21"/>
     </row>
-    <row r="122" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L122" s="21"/>
     </row>
-    <row r="123" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L123" s="21"/>
     </row>
-    <row r="124" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L124" s="21"/>
     </row>
-    <row r="126" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L126" s="21"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
primeiros testes da função de achar offset
</commit_message>
<xml_diff>
--- a/Data/A320_inputs.xlsx
+++ b/Data/A320_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giparoli\Documents\Projetos\AEco\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC492D32-BC10-4566-A32A-7B49CD6DFC0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7445A3D3-183D-4CB7-A3A0-2B88B67245C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1608,8 +1608,8 @@
   <dimension ref="A1:L122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2268,15 +2268,15 @@
         <v>21</v>
       </c>
       <c r="C30" s="19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D30" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E30" s="19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9" t="s">
@@ -2310,15 +2310,15 @@
         <v>23</v>
       </c>
       <c r="C32" s="19">
-        <v>1.0000000000000001E-5</v>
+        <v>0.5</v>
       </c>
       <c r="D32" s="19">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>0.5</v>
       </c>
       <c r="E32" s="19">
         <f t="shared" si="1"/>
-        <v>1.0000000000000001E-5</v>
+        <v>0.5</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9" t="s">

</xml_diff>